<commit_message>
Version 2: Finish testing with 7 cases with actual output and case report
</commit_message>
<xml_diff>
--- a/manipulating-test-cases.xlsx
+++ b/manipulating-test-cases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jarvinia\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\Term 1\CPR 101\Final Project\Manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED4ED82-6BF9-4420-B761-A6E30D3FFD3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3BE58D-053E-4E30-9747-C6E6F671F078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -776,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A19" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
       <text>
         <r>
           <rPr>
@@ -820,7 +820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
       <text>
         <r>
           <rPr>
@@ -885,7 +885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C19" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
       <text>
         <r>
           <rPr>
@@ -911,7 +911,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
       <text>
         <r>
           <rPr>
@@ -956,7 +956,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E19" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
       <text>
         <r>
           <rPr>
@@ -980,7 +980,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -1003,7 +1003,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G19" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -1023,7 +1023,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
   <si>
     <t>Comments</t>
   </si>
@@ -1178,9 +1178,6 @@
     <t>concatenate()</t>
   </si>
   <si>
-    <t>string1="John" string2=" Smith"</t>
-  </si>
-  <si>
     <t>John Smith</t>
   </si>
   <si>
@@ -1194,9 +1191,6 @@
   </si>
   <si>
     <t>string1="Hello this is John Smith," string2=" Nice to meet you!"</t>
-  </si>
-  <si>
-    <t>string1="Hi John Smith" string2=" Nice to meet you!"</t>
   </si>
   <si>
     <t>Jarvinia Zhao
@@ -1212,9 +1206,6 @@
     <t>empty</t>
   </si>
   <si>
-    <t>string1=""(empty) string2=""(empty)</t>
-  </si>
-  <si>
     <t>string1="Hello this is John Smith, Nice to meet you!"</t>
   </si>
   <si>
@@ -1260,6 +1251,102 @@
   <si>
     <t>Hello this is John Smith, Nice to meet you! 
 (Buffer overflow)</t>
+  </si>
+  <si>
+    <t>Jarvinia Zhao
+11-30-2023</t>
+  </si>
+  <si>
+    <t>comparison()</t>
+  </si>
+  <si>
+    <t>+ Test the equal condition, the 2 string are identical</t>
+  </si>
+  <si>
+    <t>compare1="test"  
+compare2="test"</t>
+  </si>
+  <si>
+    <t>+ Test first string is less than second string/ Case sensitive</t>
+  </si>
+  <si>
+    <t>compare1="Test"  
+compare2="test"</t>
+  </si>
+  <si>
+    <t>"Test" string is less than "test"</t>
+  </si>
+  <si>
+    <t>"test" string is equal to "test"</t>
+  </si>
+  <si>
+    <t>+ Compare both empty string</t>
+  </si>
+  <si>
+    <t>+ Test the length of string with same beginning characters</t>
+  </si>
+  <si>
+    <t>compare1="Hello World"  
+compare2="Hello"</t>
+  </si>
+  <si>
+    <t>"Hello World" string is greater than "Hello"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare1="" (empty) 
+compare2="" (empty) </t>
+  </si>
+  <si>
+    <t>""  string is equal to ""</t>
+  </si>
+  <si>
+    <t>+ Compare the special charaters</t>
+  </si>
+  <si>
+    <t>- Over-the-edge: the first string length is longer than the buffer size</t>
+  </si>
+  <si>
+    <t>compare1="Hello this is John Smith, Nice to meet you!"  
+compare2="Hello this is John Smith"</t>
+  </si>
+  <si>
+    <t>Unable to input compare2 and compare1 should be truncated to BUFFER_SIZE -1 and the rest data will store in compare2 ("Hello this is John Smith, Nice" string is less than "to meet you!")</t>
+  </si>
+  <si>
+    <t>- Over-the-edge: the first string is just reaching the edge and the second string length is longer than the buffer size. Except the length, they have idential content</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare1="Hello this is John Smith, Nice"  
+compare2="Hello this is John Smith, Nice to meet you!"  </t>
+  </si>
+  <si>
+    <t>compare1="@123"  
+compare2="$456"</t>
+  </si>
+  <si>
+    <t>"@123" string is greater than "$456"</t>
+  </si>
+  <si>
+    <t>Recommendation: Manually check the compare2 length after uer input, if user exceed the limit prompt an error message and let the user input again</t>
+  </si>
+  <si>
+    <t>Recommendation: Manually check the compare1 length after uer input, if user exceed the limit prompt an error message and let the user input again OR if the program will tale the truncated input from compare1, a clean buffer function should be called after input of compare1 to allow input of compare2</t>
+  </si>
+  <si>
+    <t>compare2 should be truncated to BUFFER_SIZE-1, and the output should be compare1 and compare2 is same ("Hello this is John Smith, Nice" string is equal to "Hello this is John Smith, Nice")
+Can input the next compare1 value</t>
+  </si>
+  <si>
+    <t>string1="John" 
+string2=" Smith"</t>
+  </si>
+  <si>
+    <t>string1=""(empty) 
+string2=""(empty)</t>
+  </si>
+  <si>
+    <t>string1="Hi John Smith" 
+string2=" Nice to meet you!"</t>
   </si>
 </sst>
 </file>
@@ -1650,7 +1737,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1789,6 +1876,9 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2351,10 +2441,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2396,7 +2486,7 @@
         <v>11</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2427,13 +2517,13 @@
         <v>38</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>40</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="25" t="s">
@@ -2446,13 +2536,13 @@
         <v>38</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="25" t="s">
@@ -2465,13 +2555,13 @@
         <v>38</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>45</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="25" t="s">
@@ -2484,22 +2574,22 @@
         <v>38</v>
       </c>
       <c r="B7" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="23" t="s">
-        <v>51</v>
-      </c>
       <c r="D7" s="23" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
@@ -2507,22 +2597,22 @@
         <v>38</v>
       </c>
       <c r="B8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="D8" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>55</v>
-      </c>
-      <c r="D8" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>58</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="125.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2530,22 +2620,22 @@
         <v>38</v>
       </c>
       <c r="B9" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="C9" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="23" t="s">
-        <v>57</v>
-      </c>
       <c r="E9" s="23" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2560,7 +2650,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2586,85 +2676,175 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
-      <c r="B12" s="29"/>
+    <row r="12" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="E12" s="3"/>
-      <c r="F12" s="25"/>
-    </row>
-    <row r="13" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28"/>
-      <c r="B13" s="29"/>
+      <c r="F12" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>67</v>
+      </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="25"/>
-    </row>
-    <row r="14" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="28"/>
-      <c r="B14" s="29"/>
+      <c r="F13" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>72</v>
+      </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="25"/>
-    </row>
-    <row r="15" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="28"/>
-      <c r="B15" s="29"/>
+      <c r="F14" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="25"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
-      <c r="B16" s="29"/>
+      <c r="F15" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="25"/>
-    </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="28"/>
-      <c r="B17" s="29"/>
+      <c r="F16" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="87.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="25"/>
-    </row>
-    <row r="18" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="43" t="s">
+      <c r="F17" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="113" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="28" t="s">
+        <v>62</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="20" t="s">
+      <c r="B19" s="44"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G18" s="37" t="s">
+      <c r="G19" s="37" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="40" t="s">
+    <row r="20" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B20" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C20" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D20" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E20" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F20" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G20" s="22" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
-      <c r="B20" s="29"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="25"/>
     </row>
     <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
@@ -2714,11 +2894,17 @@
       <c r="E28" s="3"/>
       <c r="F28" s="25"/>
     </row>
+    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="28"/>
+      <c r="B29" s="29"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="25"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F1048576">

</xml_diff>

<commit_message>
Version 1&2: Correct typos and revise the wording
</commit_message>
<xml_diff>
--- a/manipulating-test-cases.xlsx
+++ b/manipulating-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\Term 1\CPR 101\Final Project\Manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A3BE58D-053E-4E30-9747-C6E6F671F078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A171858-50C1-4F6E-9479-B45F5046F9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1175,9 +1175,6 @@
     <t>manipulating</t>
   </si>
   <si>
-    <t>concatenate()</t>
-  </si>
-  <si>
     <t>John Smith</t>
   </si>
   <si>
@@ -1206,9 +1203,6 @@
     <t>empty</t>
   </si>
   <si>
-    <t>string1="Hello this is John Smith, Nice to meet you!"</t>
-  </si>
-  <si>
     <t>- Over-the-edge: string2 exceeding max length(32)</t>
   </si>
   <si>
@@ -1219,33 +1213,10 @@
     <t>- Over-the-edge: length of each string is within buffer size but exceeding max length(32) after the concatenation</t>
   </si>
   <si>
-    <t>string1="12345" string2="Hi John Smith Nice to meet you!"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">output should be truncated: (12345Hi John Smith Nice to mee)
-or display an error message </t>
-  </si>
-  <si>
-    <t xml:space="preserve">output should be truncated (Hello this is John Smith, Nice)
- or display an error message </t>
-  </si>
-  <si>
     <t>12345Hi John Smith Nice to meet you 
 (fgets size limitation + buffer overflow)</t>
   </si>
   <si>
-    <t>fgets function truncated the string2 input base on the buffer size, however the combined string after strcat function leading to the buffer overflow
-Recommendation: Manually check the string2 length after uer input, if user exceed the limit prompt an error message and let the user input again</t>
-  </si>
-  <si>
-    <t>fgets function only reads BUFFER_SIZE -1 characters and will leave rest of characters in the input buffer.  Then when string2 call fgets function again, it read from input buffer directly. Also will has buffer overflow
-Recommendation: Manually check the string1 length after uer input, if user exceed the limit prompt an error message and let the user input again</t>
-  </si>
-  <si>
-    <t>In C, system strcat fucntion didn’t check the size of destination buffer(string1) automatically. It will simply append second string to the destination and past the end of buffer, leading to buffer overflow.This overflow can corrupt adjacent memory but might not immediately cause a crash.
-Recommendation: Manually check the combined length of string is not greater than the buffer size before call strcat function, and if the combined string exceeds the limit, prompt an error message</t>
-  </si>
-  <si>
     <t>Unable to input string2 and concatenated string1 should be truncated (Hello this is John Smith, Nice)</t>
   </si>
   <si>
@@ -1257,9 +1228,6 @@
 11-30-2023</t>
   </si>
   <si>
-    <t>comparison()</t>
-  </si>
-  <si>
     <t>+ Test the equal condition, the 2 string are identical</t>
   </si>
   <si>
@@ -1327,16 +1295,6 @@
     <t>"@123" string is greater than "$456"</t>
   </si>
   <si>
-    <t>Recommendation: Manually check the compare2 length after uer input, if user exceed the limit prompt an error message and let the user input again</t>
-  </si>
-  <si>
-    <t>Recommendation: Manually check the compare1 length after uer input, if user exceed the limit prompt an error message and let the user input again OR if the program will tale the truncated input from compare1, a clean buffer function should be called after input of compare1 to allow input of compare2</t>
-  </si>
-  <si>
-    <t>compare2 should be truncated to BUFFER_SIZE-1, and the output should be compare1 and compare2 is same ("Hello this is John Smith, Nice" string is equal to "Hello this is John Smith, Nice")
-Can input the next compare1 value</t>
-  </si>
-  <si>
     <t>string1="John" 
 string2=" Smith"</t>
   </si>
@@ -1347,6 +1305,56 @@
   <si>
     <t>string1="Hi John Smith" 
 string2=" Nice to meet you!"</t>
+  </si>
+  <si>
+    <t>string1="Hello this is John Smith, Nice to meet you!"
+string2="abc"</t>
+  </si>
+  <si>
+    <t>string1="12345" 
+string2="Hi John Smith Nice to meet you!"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output should be truncated (Hello this is John Smith, Nice)
+OR display an error message </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Output should be truncated: (12345Hi John Smith Nice to mee)
+OR display an error message </t>
+  </si>
+  <si>
+    <t>compare2 should be truncated to BUFFER_SIZE-1, and the output should be compare1 and compare2 is same ("Hello this is John Smith, Nice" string is equal to "Hello this is John Smith, Nice")
+Can't input the next compare1 value</t>
+  </si>
+  <si>
+    <t>String concatenate:
+strcat()</t>
+  </si>
+  <si>
+    <t>String comparison: 
+strcmp()</t>
+  </si>
+  <si>
+    <t>Cause: In C, system strcat fucntion didn’t check the size of destination buffer(string1) automatically. It will simply append second string to the destination and past the end of buffer, leading to buffer overflow.This overflow can corrupt adjacent memory but might not immediately cause a crash.
+Recommendation: Manually check the combined length of string is not greater than the buffer size before call strcat function, and if the combined string exceeds the limit, prompt an error message</t>
+  </si>
+  <si>
+    <t>Cause: fgets function truncated the string2 input base on the buffer size, however the combined string after strcat function leading to the buffer overflow
+Recommendation: Manually check the string2 length after uer input, if user exceed the limit prompt an error message and let the user input again</t>
+  </si>
+  <si>
+    <t>Causes: fgets function only reads BUFFER_SIZE -1 characters and will leave rest of characters in the input buffer.  Then when string2 call fgets function again, it read from input buffer directly. Also will has buffer overflow
+Recommendation: Manually check the string1 length after uer input, if user exceed the limit prompt an error message and let the user input again</t>
+  </si>
+  <si>
+    <t>Causes: fgets size limitation (detail can refer to G7)
+Recommendation: Manually check the compare1 length after uer input, if user exceed the limit prompt an error message and let the user input again 
+OR if the program will take the truncated input from compare1, a clean buffer function should be called after input of compare1 to allow input of compare2</t>
+  </si>
+  <si>
+    <t>Causes: fgets size limitation (detail can refer to G7)
+Recommendation: Manually check the compare2 length after uer input, if user exceed the limit prompt an error message and let the user input again
+OR if the program will take the truncated input from compare2, a clean buffer function should be called after input of compare2 to allow input of next compare1</t>
   </si>
 </sst>
 </file>
@@ -1865,6 +1873,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1876,9 +1887,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2238,22 +2246,22 @@
       <c r="B1" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="45" t="str">
+      <c r="C1" s="46" t="str">
         <f>"Do not save or use this worksheet – sample test cases only"</f>
         <v>Do not save or use this worksheet – sample test cases only</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
       <c r="E2" s="31"/>
       <c r="F2" s="18" t="s">
         <v>11</v>
@@ -2443,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2465,28 +2473,28 @@
       <c r="B1" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="45" t="str">
+      <c r="C1" s="46" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As manipulating_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
     </row>
     <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2514,16 +2522,16 @@
     </row>
     <row r="4" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="23" t="s">
         <v>38</v>
-      </c>
-      <c r="B4" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>39</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="25" t="s">
@@ -2533,16 +2541,16 @@
     </row>
     <row r="5" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="25" t="s">
@@ -2550,18 +2558,18 @@
       </c>
       <c r="G5" s="26"/>
     </row>
-    <row r="6" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="25" t="s">
@@ -2569,88 +2577,88 @@
       </c>
       <c r="G6" s="26"/>
     </row>
-    <row r="7" spans="1:7" ht="100" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>48</v>
+        <v>77</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>53</v>
+        <v>80</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="125.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="138" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>38</v>
+        <v>82</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44"/>
-      <c r="D10" s="44"/>
-      <c r="E10" s="44"/>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="37" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2677,17 +2685,17 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B12" s="47" t="s">
-        <v>63</v>
+      <c r="A12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" s="43" t="s">
+        <v>54</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="25" t="s">
@@ -2695,17 +2703,17 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="47" t="s">
-        <v>65</v>
+      <c r="A13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="43" t="s">
+        <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="25" t="s">
@@ -2713,109 +2721,109 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="47" t="s">
-        <v>70</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="47" t="s">
-        <v>69</v>
+    <row r="15" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="43" t="s">
+        <v>60</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A16" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="47" t="s">
-        <v>75</v>
+    <row r="16" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="43" t="s">
+        <v>66</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="87.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="47" t="s">
-        <v>76</v>
+    <row r="17" spans="1:7" ht="100" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>67</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="113" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B18" s="47" t="s">
-        <v>79</v>
+      <c r="A18" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B18" s="43" t="s">
+        <v>70</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="43" t="s">
+      <c r="A19" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="44"/>
-      <c r="C19" s="44"/>
-      <c r="D19" s="44"/>
-      <c r="E19" s="44"/>
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45"/>
+      <c r="E19" s="45"/>
       <c r="F19" s="20" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Version 3: Upload testing case records, and modify the format of testing.txt
</commit_message>
<xml_diff>
--- a/manipulating-test-cases.xlsx
+++ b/manipulating-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\Term 1\CPR 101\Final Project\Manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A171858-50C1-4F6E-9479-B45F5046F9A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B7E959-FB05-4E5D-876B-1286078D0804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -776,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
+    <comment ref="A21" authorId="0" shapeId="0" xr:uid="{C02017E4-821F-4A2D-86D8-AB6EEDB22A86}">
       <text>
         <r>
           <rPr>
@@ -820,7 +820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
+    <comment ref="B21" authorId="0" shapeId="0" xr:uid="{05B2FD82-D89E-4CA6-B9CD-DADA87D3459D}">
       <text>
         <r>
           <rPr>
@@ -885,7 +885,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
+    <comment ref="C21" authorId="0" shapeId="0" xr:uid="{23C8660F-F760-4D26-A851-EB73153BFF94}">
       <text>
         <r>
           <rPr>
@@ -911,7 +911,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{D011BF0E-2314-4932-9D14-810DC408E97A}">
       <text>
         <r>
           <rPr>
@@ -956,7 +956,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
+    <comment ref="E21" authorId="0" shapeId="0" xr:uid="{135F8B3A-CCD4-4CA6-9ADB-2D061B1E1D5D}">
       <text>
         <r>
           <rPr>
@@ -980,7 +980,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{CDD09690-9535-4ED1-A265-0F0404D34131}">
       <text>
         <r>
           <rPr>
@@ -1003,7 +1003,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
+    <comment ref="G21" authorId="0" shapeId="0" xr:uid="{508032F0-07F6-4EDA-A011-0A700A6AF801}">
       <text>
         <r>
           <rPr>
@@ -1023,7 +1023,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="127">
   <si>
     <t>Comments</t>
   </si>
@@ -1352,16 +1352,151 @@
 OR if the program will take the truncated input from compare1, a clean buffer function should be called after input of compare1 to allow input of compare2</t>
   </si>
   <si>
+    <t>String search:
+strstr()</t>
+  </si>
+  <si>
+    <t>haysteck = "Hello World!"
+needle = "World“</t>
+  </si>
+  <si>
+    <t>haysteck = "Test starts now right?"
+needle = "Test“</t>
+  </si>
+  <si>
+    <t>haysteck = "Hello World!"
+needle = "o“</t>
+  </si>
+  <si>
+    <t>haysteck = "This is a test"
+needle = "test“</t>
+  </si>
+  <si>
+    <t>haysteck = "Hello World!"
+needle = "Happy“</t>
+  </si>
+  <si>
+    <t>- Over-the-edge: needle(the second string) exceed the buffer size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Empty needle (the second string) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Normal case: haystack (the first string)  contains needle (the second string) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ haystack (the first string) contains needle and needle (the second string)  at beginning </t>
+  </si>
+  <si>
+    <t>'+ haystack (the first string) contains needle and needle (the second string)  at end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ haystack (the first string) contains needle and needle (the second string)  is a single character </t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Normal case: haystack (the first string) doesn't contains needle (the second string) </t>
+  </si>
+  <si>
+    <t>+ Empty haystack (the first string)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+ Empty haystack (the first string) and needle (the second string) </t>
+  </si>
+  <si>
+    <t>- Over-the-edge: haystack (the first string) exceed the buffer size</t>
+  </si>
+  <si>
+    <t>haysteck = "four"
+needle = "one two three four five six seven eight nine ten" (48 characters)</t>
+  </si>
+  <si>
+    <t>haysteck = "one two three four five six seven eight nine ten" (48 characters)
+needle = "six“</t>
+  </si>
+  <si>
+    <t>“World” found at 6 position</t>
+  </si>
+  <si>
+    <t>Test found at 0 position</t>
+  </si>
+  <si>
+    <t>test found at 10 position</t>
+  </si>
+  <si>
+    <t>o found at 4 position</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> found at 0 position</t>
+  </si>
+  <si>
+    <t>haysteck = "" (empty)
+needle = "“ (empty)</t>
+  </si>
+  <si>
+    <t>haysteck = "" (empty)
+needle = "test“</t>
+  </si>
+  <si>
+    <t>haysteck = "test"
+needle = "“ (empty)</t>
+  </si>
+  <si>
+    <t>- Over-the-edge: haystack (the first string) exceed the buffer size, but haystack contains a repeated pattern</t>
+  </si>
+  <si>
+    <t>haysteck = "two three four two three four two three four two three four" (59 characters)
+needle = "two“</t>
+  </si>
+  <si>
+    <t>Unable to input needle. haystack should be truncated to BUFFER_SIZE -1 and the rest data will store in needle
+output: Not found</t>
+  </si>
+  <si>
+    <t>Can't input the next haystack value
+Output: Not found</t>
+  </si>
+  <si>
     <t>Causes: fgets size limitation (detail can refer to G7)
-Recommendation: Manually check the compare2 length after uer input, if user exceed the limit prompt an error message and let the user input again
+Recommendation: Manually check the compare2 length after user input, if user exceed the limit prompt an error message and let the user input again
 OR if the program will take the truncated input from compare2, a clean buffer function should be called after input of compare2 to allow input of next compare1</t>
+  </si>
+  <si>
+    <t>Causes: fgets prevent buffer overflow and also limit the input size store in variable haystack
+Recommendation: Manually check haystack length after user input. if user exceed the limit prompt an error message and let the user input again</t>
+  </si>
+  <si>
+    <t>Causes: fgets prevent buffer overflow and also limit the input size store in variable haystack. In this special senario, even though the entire haystack doesn't fit into the buffer, the needle is still found because it is contained within the part of the haystack that fits into the buffer. 
+Recommendation: Manually check haystack length after user input. if user exceed the limit prompt an error message and let the user input again</t>
+  </si>
+  <si>
+    <t>Causes: fgets prevent buffer overflow and also limit the input size store in variable needle
+Recommendation: Manually check the needle length after user input, if user exceed the limit prompt an error message and let the user input again
+OR if the program will take the truncated input from needle, a clean buffer function should be called after input of needle to allow input of next haystack</t>
+  </si>
+  <si>
+    <t>Unable to input needle. haystack should be truncated to BUFFER_SIZE -1 and the rest data will store in needle. BUT result may vary in different senarios</t>
+  </si>
+  <si>
+    <t>Needle is found in haystack with this reapted pattern
+Output:
+"wo three four two three four" found at 1 position</t>
+  </si>
+  <si>
+    <t>+ Compare one empty string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compare1="" (empty) 
+compare2="test"  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1379,13 +1514,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <color indexed="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1738,14 +1866,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1762,13 +1886,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1783,10 +1907,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1801,7 +1925,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1813,10 +1937,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1825,37 +1949,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="16" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="15" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1876,22 +1994,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="6">
     <dxf>
@@ -2243,26 +2363,26 @@
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="46" t="str">
+      <c r="C1" s="44" t="str">
         <f>"Do not save or use this worksheet – sample test cases only"</f>
         <v>Do not save or use this worksheet – sample test cases only</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="31"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="29"/>
       <c r="F2" s="18" t="s">
         <v>11</v>
       </c>
@@ -2306,7 +2426,7 @@
       <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="32"/>
+      <c r="E4" s="30"/>
       <c r="F4" s="9" t="s">
         <v>27</v>
       </c>
@@ -2326,7 +2446,7 @@
       <c r="D5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="33"/>
+      <c r="E5" s="31"/>
       <c r="F5" s="10" t="s">
         <v>27</v>
       </c>
@@ -2346,7 +2466,7 @@
       <c r="D6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="33"/>
+      <c r="E6" s="31"/>
       <c r="F6" s="10" t="s">
         <v>27</v>
       </c>
@@ -2366,7 +2486,7 @@
       <c r="D7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="32"/>
       <c r="F7" s="10" t="s">
         <v>27</v>
       </c>
@@ -2386,8 +2506,8 @@
       <c r="D8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E8" s="32"/>
-      <c r="F8" s="30" t="s">
+      <c r="E8" s="30"/>
+      <c r="F8" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="13" t="s">
@@ -2408,8 +2528,8 @@
       <c r="D9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="32"/>
-      <c r="F9" s="30" t="s">
+      <c r="E9" s="30"/>
+      <c r="F9" s="28" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="13" t="s">
@@ -2449,10 +2569,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2467,56 +2587,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="46" t="str">
+      <c r="C1" s="44" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As manipulating_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47"/>
-      <c r="G1" s="47"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
       <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="35" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="39" t="s">
+      <c r="G3" s="37" t="s">
         <v>0</v>
       </c>
     </row>
@@ -2647,34 +2767,34 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="44" t="s">
+      <c r="A10" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
       <c r="F10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="37" t="s">
+      <c r="G10" s="35" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="42" t="s">
+      <c r="C11" s="40" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="E11" s="40" t="s">
         <v>18</v>
       </c>
       <c r="F11" s="21" t="s">
@@ -2688,7 +2808,7 @@
       <c r="A12" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B12" s="43" t="s">
+      <c r="B12" s="41" t="s">
         <v>54</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -2706,7 +2826,7 @@
       <c r="A13" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="43" t="s">
+      <c r="B13" s="41" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -2724,7 +2844,7 @@
       <c r="A14" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="41" t="s">
         <v>61</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -2742,14 +2862,11 @@
       <c r="A15" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="43" t="s">
-        <v>60</v>
+      <c r="B15" s="41" t="s">
+        <v>125</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>65</v>
+        <v>126</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="25" t="s">
@@ -2760,159 +2877,330 @@
       <c r="A16" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="43" t="s">
-        <v>66</v>
+      <c r="B16" s="41" t="s">
+        <v>60</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="25" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="100" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B17" s="43" t="s">
-        <v>67</v>
+      <c r="B17" s="41" t="s">
+        <v>66</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="113" thickBot="1" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="100" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="43" t="s">
-        <v>70</v>
+      <c r="B18" s="41" t="s">
+        <v>67</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="113" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="42" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G20" s="35" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="40" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="50" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="45"/>
-      <c r="C19" s="45"/>
-      <c r="D19" s="45"/>
-      <c r="E19" s="45"/>
-      <c r="F19" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" s="42" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>1</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="28"/>
-      <c r="B21" s="29"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="25"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="28"/>
-      <c r="B22" s="29"/>
+      <c r="B22" s="46" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="E22" s="3"/>
-      <c r="F22" s="25"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="29"/>
+      <c r="F22" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="50" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B23" s="46" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="25"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="29"/>
+      <c r="F23" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="50" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="25"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="29"/>
+      <c r="F24" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>109</v>
+      </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="25"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="29"/>
+      <c r="F25" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="E26" s="3"/>
-      <c r="F26" s="25"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="29"/>
+      <c r="F26" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>110</v>
+      </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="25"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="28"/>
-      <c r="B28" s="29"/>
+      <c r="F27" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="25"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="28"/>
-      <c r="B29" s="29"/>
+      <c r="F28" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="46" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>111</v>
+      </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="25"/>
+      <c r="F29" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="41" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="125" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>122</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="A10:E10"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
     <mergeCell ref="C1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="F4:F1048576">

</xml_diff>

<commit_message>
Version 2: Add one more testing case - one empty string
</commit_message>
<xml_diff>
--- a/manipulating-test-cases.xlsx
+++ b/manipulating-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\Term 1\CPR 101\Final Project\Manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B7E959-FB05-4E5D-876B-1286078D0804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCEB78E-8297-4564-9DB2-1FDCED74E24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1023,7 +1023,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="128">
   <si>
     <t>Comments</t>
   </si>
@@ -1200,9 +1200,6 @@
     <t>- Over-the-edge: string1 exceeding max length(32)</t>
   </si>
   <si>
-    <t>empty</t>
-  </si>
-  <si>
     <t>- Over-the-edge: string2 exceeding max length(32)</t>
   </si>
   <si>
@@ -1490,6 +1487,12 @@
   <si>
     <t xml:space="preserve">compare1="" (empty) 
 compare2="test"  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> string is less than "test"</t>
+  </si>
+  <si>
+    <t>(empty)</t>
   </si>
 </sst>
 </file>
@@ -2571,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2642,13 +2645,13 @@
     </row>
     <row r="4" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="24" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>38</v>
@@ -2661,16 +2664,16 @@
     </row>
     <row r="5" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B5" s="24" t="s">
         <v>41</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>46</v>
+        <v>127</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="25" t="s">
@@ -2680,13 +2683,13 @@
     </row>
     <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="24" t="s">
         <v>40</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D6" s="23" t="s">
         <v>44</v>
@@ -2699,71 +2702,71 @@
     </row>
     <row r="7" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="24" t="s">
         <v>45</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="138" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C9" s="23" t="s">
         <v>42</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2778,7 +2781,7 @@
         <v>11</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2806,16 +2809,16 @@
     </row>
     <row r="12" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="25" t="s">
@@ -2824,16 +2827,16 @@
     </row>
     <row r="13" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="25" t="s">
@@ -2842,16 +2845,16 @@
     </row>
     <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B14" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="25" t="s">
@@ -2860,12 +2863,15 @@
     </row>
     <row r="15" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="D15" s="3" t="s">
         <v>126</v>
       </c>
       <c r="E15" s="3"/>
@@ -2875,16 +2881,16 @@
     </row>
     <row r="16" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="25" t="s">
@@ -2893,16 +2899,16 @@
     </row>
     <row r="17" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="25" t="s">
@@ -2911,44 +2917,44 @@
     </row>
     <row r="18" spans="1:7" ht="100" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B18" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="113" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2991,16 +2997,16 @@
     </row>
     <row r="22" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B22" s="46" t="s">
+        <v>95</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>89</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="25" t="s">
@@ -3009,16 +3015,16 @@
     </row>
     <row r="23" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B23" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="25" t="s">
@@ -3027,16 +3033,16 @@
     </row>
     <row r="24" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="25" t="s">
@@ -3045,16 +3051,16 @@
     </row>
     <row r="25" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B25" s="46" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="25" t="s">
@@ -3063,16 +3069,16 @@
     </row>
     <row r="26" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B26" s="46" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="25" t="s">
@@ -3081,16 +3087,16 @@
     </row>
     <row r="27" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B27" s="46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="25" t="s">
@@ -3099,16 +3105,16 @@
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B28" s="46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="25" t="s">
@@ -3117,16 +3123,16 @@
     </row>
     <row r="29" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="46" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="25" t="s">
@@ -3135,65 +3141,65 @@
     </row>
     <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="125" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B31" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>116</v>
-      </c>
       <c r="D31" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Version3: Minor format modifications
</commit_message>
<xml_diff>
--- a/manipulating-test-cases.xlsx
+++ b/manipulating-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\Term 1\CPR 101\Final Project\Manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCEB78E-8297-4564-9DB2-1FDCED74E24D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E394C59-76A2-40D8-B6F6-88C5091F2884}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1168,10 +1168,6 @@
     <t>Sample Test Cases</t>
   </si>
   <si>
-    <t>????? Tester's Name ?????
-????? Date ?????</t>
-  </si>
-  <si>
     <t>manipulating</t>
   </si>
   <si>
@@ -1448,14 +1444,6 @@
 needle = "two“</t>
   </si>
   <si>
-    <t>Unable to input needle. haystack should be truncated to BUFFER_SIZE -1 and the rest data will store in needle
-output: Not found</t>
-  </si>
-  <si>
-    <t>Can't input the next haystack value
-Output: Not found</t>
-  </si>
-  <si>
     <t>Causes: fgets size limitation (detail can refer to G7)
 Recommendation: Manually check the compare2 length after user input, if user exceed the limit prompt an error message and let the user input again
 OR if the program will take the truncated input from compare2, a clean buffer function should be called after input of compare2 to allow input of next compare1</t>
@@ -1493,6 +1481,18 @@
   </si>
   <si>
     <t>(empty)</t>
+  </si>
+  <si>
+    <t>Jarvinia Zhao
+12-03-2023</t>
+  </si>
+  <si>
+    <t>Unable to input needle. haystack should be truncated to BUFFER_SIZE -1 and the rest data will store in needle
+Expected output: Not found</t>
+  </si>
+  <si>
+    <t>Can't input the next haystack value
+Expected Output: Not found</t>
   </si>
 </sst>
 </file>
@@ -1997,6 +1997,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2008,9 +2011,6 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2369,22 +2369,22 @@
       <c r="B1" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="44" t="str">
+      <c r="C1" s="45" t="str">
         <f>"Do not save or use this worksheet – sample test cases only"</f>
         <v>Do not save or use this worksheet – sample test cases only</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="29"/>
       <c r="F2" s="18" t="s">
         <v>11</v>
@@ -2574,8 +2574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{489FCF92-76BB-4101-9D49-11677A4362B7}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2594,30 +2594,30 @@
         <v>9</v>
       </c>
       <c r="B1" s="34" t="s">
-        <v>37</v>
-      </c>
-      <c r="C1" s="44" t="str">
+        <v>36</v>
+      </c>
+      <c r="C1" s="45" t="str">
         <f>"Save As " &amp; B1  &amp; "_test_cases.xlsx"</f>
         <v>Save As manipulating_test_cases.xlsx</v>
       </c>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
     </row>
     <row r="2" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
       <c r="F2" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2645,16 +2645,16 @@
     </row>
     <row r="4" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="25" t="s">
@@ -2664,16 +2664,16 @@
     </row>
     <row r="5" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="25" t="s">
@@ -2683,16 +2683,16 @@
     </row>
     <row r="6" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="25" t="s">
@@ -2702,86 +2702,86 @@
     </row>
     <row r="7" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D7" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="23" t="s">
         <v>50</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>51</v>
       </c>
       <c r="F7" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G7" s="26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="87.5" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F8" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="138" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
       <c r="F10" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2809,16 +2809,16 @@
     </row>
     <row r="12" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B12" s="41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>54</v>
-      </c>
       <c r="D12" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="25" t="s">
@@ -2827,16 +2827,16 @@
     </row>
     <row r="13" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="25" t="s">
@@ -2845,16 +2845,16 @@
     </row>
     <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B14" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="25" t="s">
@@ -2863,16 +2863,16 @@
     </row>
     <row r="15" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="25" t="s">
@@ -2881,16 +2881,16 @@
     </row>
     <row r="16" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="25" t="s">
@@ -2899,16 +2899,16 @@
     </row>
     <row r="17" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="25" t="s">
@@ -2917,59 +2917,59 @@
     </row>
     <row r="18" spans="1:7" ht="100" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B18" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="113" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B19" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="25" t="s">
         <v>7</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="42" t="s">
+      <c r="A20" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43"/>
-      <c r="E20" s="43"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="44"/>
+      <c r="E20" s="44"/>
       <c r="F20" s="20" t="s">
         <v>11</v>
       </c>
       <c r="G20" s="35" t="s">
-        <v>36</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2997,16 +2997,16 @@
     </row>
     <row r="22" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B22" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B22" s="46" t="s">
-        <v>95</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="D22" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="25" t="s">
@@ -3015,16 +3015,16 @@
     </row>
     <row r="23" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B23" s="46" t="s">
-        <v>96</v>
+        <v>86</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>95</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E23" s="3"/>
       <c r="F23" s="25" t="s">
@@ -3033,16 +3033,16 @@
     </row>
     <row r="24" spans="1:7" ht="50" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B24" s="46" t="s">
-        <v>97</v>
+        <v>86</v>
+      </c>
+      <c r="B24" s="42" t="s">
+        <v>96</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="25" t="s">
@@ -3051,16 +3051,16 @@
     </row>
     <row r="25" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B25" s="46" t="s">
-        <v>98</v>
+        <v>86</v>
+      </c>
+      <c r="B25" s="42" t="s">
+        <v>97</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="25" t="s">
@@ -3069,16 +3069,16 @@
     </row>
     <row r="26" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B26" s="46" t="s">
-        <v>99</v>
+        <v>86</v>
+      </c>
+      <c r="B26" s="42" t="s">
+        <v>98</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E26" s="3"/>
       <c r="F26" s="25" t="s">
@@ -3087,16 +3087,16 @@
     </row>
     <row r="27" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="46" t="s">
-        <v>100</v>
+        <v>86</v>
+      </c>
+      <c r="B27" s="42" t="s">
+        <v>99</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E27" s="3"/>
       <c r="F27" s="25" t="s">
@@ -3105,16 +3105,16 @@
     </row>
     <row r="28" spans="1:7" ht="25" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B28" s="46" t="s">
-        <v>94</v>
+        <v>86</v>
+      </c>
+      <c r="B28" s="42" t="s">
+        <v>93</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="25" t="s">
@@ -3123,16 +3123,16 @@
     </row>
     <row r="29" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" s="46" t="s">
-        <v>101</v>
+        <v>86</v>
+      </c>
+      <c r="B29" s="42" t="s">
+        <v>100</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="25" t="s">
@@ -3141,65 +3141,65 @@
     </row>
     <row r="30" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B30" s="41" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>116</v>
+        <v>126</v>
       </c>
       <c r="F30" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="125" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B31" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="D31" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F31" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" s="41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>117</v>
+        <v>127</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>7</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor modifications for recovering
</commit_message>
<xml_diff>
--- a/manipulating-test-cases.xlsx
+++ b/manipulating-test-cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Seneca\Term 1\CPR 101\Final Project\CPR101-Final-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECF08806-349B-40AB-95CA-A0C11A5C10C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20172B37-6D02-43B1-A5D7-279E9F569537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1115,10 +1115,6 @@
 OR if the program will take the truncated input from compare2, a clean buffer function should be called after input of compare2 to allow input of next compare1</t>
   </si>
   <si>
-    <t>Causes: fgets prevent buffer overflow and also limit the input size store in variable haystack
-Recommendation: Manually check haystack length after user input. if user exceed the limit prompt an error message and let the user input again</t>
-  </si>
-  <si>
     <t>Causes: fgets prevent buffer overflow and also limit the input size store in variable haystack. In this special senario, even though the entire haystack doesn't fit into the buffer, the needle is still found because it is contained within the part of the haystack that fits into the buffer. 
 Recommendation: Manually check haystack length after user input. if user exceed the limit prompt an error message and let the user input again</t>
   </si>
@@ -1159,6 +1155,10 @@
   <si>
     <t>Can't input the next haystack value
 Expected Output: Not found</t>
+  </si>
+  <si>
+    <t>Causes: fgets prevent buffer overflow and also limit the input size store in variable haystack.
+Recommendation: Manually check haystack length after user input. if user exceed the limit prompt an error message and let the user input again</t>
   </si>
 </sst>
 </file>
@@ -1801,7 +1801,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1899,7 +1899,7 @@
         <v>51</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E5" s="7"/>
       <c r="F5" s="9" t="s">
@@ -2092,13 +2092,13 @@
         <v>59</v>
       </c>
       <c r="B15" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="9" t="s">
@@ -2195,7 +2195,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="26.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -2376,13 +2376,13 @@
         <v>81</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="125" x14ac:dyDescent="0.25">
@@ -2396,16 +2396,16 @@
         <v>92</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="112.5" x14ac:dyDescent="0.25">
@@ -2419,13 +2419,13 @@
         <v>80</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>